<commit_message>
Update BOM_Low Profile Earcup Assy.xlsx
Added cost for AIC shield
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM_Low Profile Earcup Assy.xlsx
+++ b/Bill of Materials/BOM_Low Profile Earcup Assy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="12435" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="12435" windowHeight="7500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EARCUP_WITH PINNA" sheetId="6" r:id="rId1"/>
@@ -414,7 +414,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,12 +424,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +544,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -579,7 +573,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,15 +580,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -604,19 +597,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -662,6 +642,19 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -967,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -987,67 +980,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="49">
         <v>43566</v>
       </c>
-      <c r="C3" s="29"/>
+      <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="29"/>
-    </row>
-    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="C4" s="49"/>
+    </row>
+    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="18"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1186,7 +1179,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="11">
-        <f>I11*H11</f>
+        <f t="shared" ref="J11:J16" si="1">I11*H11</f>
         <v>3.7520000000000002</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -1223,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="11">
-        <f>I12*H12</f>
+        <f t="shared" si="1"/>
         <v>0.19519999999999998</v>
       </c>
       <c r="K12" s="9"/>
@@ -1257,7 +1250,7 @@
         <v>0.1</v>
       </c>
       <c r="J13" s="11">
-        <f>I13*H13</f>
+        <f t="shared" si="1"/>
         <v>1.3860000000000001</v>
       </c>
       <c r="K13" s="9"/>
@@ -1291,7 +1284,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="11">
-        <f>I14*H14</f>
+        <f t="shared" si="1"/>
         <v>25.94</v>
       </c>
       <c r="K14" s="9"/>
@@ -1326,10 +1319,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="11">
-        <f>I15*H15</f>
+        <f t="shared" si="1"/>
         <v>68.89</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="27" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1352,7 +1345,7 @@
       <c r="F16" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="34" t="s">
         <v>86</v>
       </c>
       <c r="H16" s="10">
@@ -1362,10 +1355,10 @@
         <v>0.1</v>
       </c>
       <c r="J16" s="11">
-        <f>I16*H16</f>
+        <f t="shared" si="1"/>
         <v>1.468</v>
       </c>
-      <c r="K16" s="28"/>
+      <c r="K16" s="27"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1374,29 +1367,29 @@
       <c r="B17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="39">
+      <c r="G17" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="31">
         <v>16.989999999999998</v>
       </c>
       <c r="I17" s="8">
         <v>2</v>
       </c>
       <c r="J17" s="11">
-        <f t="shared" ref="J17:J21" si="1">I17*H17</f>
+        <f t="shared" ref="J17:J21" si="2">I17*H17</f>
         <v>33.979999999999997</v>
       </c>
       <c r="K17" s="9"/>
@@ -1430,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.28</v>
       </c>
       <c r="K18" s="9"/>
@@ -1465,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4950000000000001</v>
       </c>
       <c r="K19" s="9"/>
@@ -1500,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.9950000000000001</v>
       </c>
       <c r="K20" s="9"/>
@@ -1521,20 +1514,20 @@
       <c r="E21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="39">
+      <c r="H21" s="31">
         <v>2.5</v>
       </c>
       <c r="I21" s="8">
         <v>1</v>
       </c>
       <c r="J21" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="K21" s="9" t="s">
@@ -1570,7 +1563,7 @@
       <c r="I22" s="8">
         <v>2</v>
       </c>
-      <c r="J22" s="48">
+      <c r="J22" s="40">
         <f>I22*H22</f>
         <v>7.333333333333333</v>
       </c>
@@ -1607,7 +1600,7 @@
       <c r="I23" s="8">
         <v>0</v>
       </c>
-      <c r="J23" s="48">
+      <c r="J23" s="40">
         <f>I23*H23</f>
         <v>0</v>
       </c>
@@ -1615,54 +1608,54 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>17</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="47">
+      <c r="H24" s="39">
         <v>1.2</v>
       </c>
-      <c r="I24" s="43">
+      <c r="I24" s="35">
         <v>4</v>
       </c>
-      <c r="J24" s="48">
+      <c r="J24" s="40">
         <f>I24*H24</f>
         <v>4.8</v>
       </c>
-      <c r="K24" s="45"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="24">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="23">
         <f xml:space="preserve"> SUM(J9:J24)</f>
         <v>420.01453333333336</v>
       </c>
@@ -1720,67 +1713,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="49">
         <v>43566</v>
       </c>
-      <c r="C3" s="29"/>
+      <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="29"/>
-    </row>
-    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="C4" s="49"/>
+    </row>
+    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="18"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1919,7 +1912,7 @@
         <v>2</v>
       </c>
       <c r="J11" s="11">
-        <f>I11*H11</f>
+        <f t="shared" ref="J11:J17" si="1">I11*H11</f>
         <v>56.7</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -1956,7 +1949,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="11">
-        <f>I12*H12</f>
+        <f t="shared" si="1"/>
         <v>3.7520000000000002</v>
       </c>
       <c r="K12" s="9" t="s">
@@ -1993,7 +1986,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="11">
-        <f>I13*H13</f>
+        <f t="shared" si="1"/>
         <v>0.19519999999999998</v>
       </c>
       <c r="K13" s="9"/>
@@ -2027,7 +2020,7 @@
         <v>0.1</v>
       </c>
       <c r="J14" s="11">
-        <f>I14*H14</f>
+        <f t="shared" si="1"/>
         <v>1.3860000000000001</v>
       </c>
       <c r="K14" s="9"/>
@@ -2061,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="11">
-        <f>I15*H15</f>
+        <f t="shared" si="1"/>
         <v>25.94</v>
       </c>
       <c r="K15" s="9"/>
@@ -2096,10 +2089,10 @@
         <v>2</v>
       </c>
       <c r="J16" s="11">
-        <f>I16*H16</f>
+        <f t="shared" si="1"/>
         <v>68.89</v>
       </c>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="27" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2122,7 +2115,7 @@
       <c r="F17" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="34" t="s">
         <v>86</v>
       </c>
       <c r="H17" s="10">
@@ -2132,10 +2125,10 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="11">
-        <f>I17*H17</f>
+        <f t="shared" si="1"/>
         <v>1.468</v>
       </c>
-      <c r="K17" s="28"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
@@ -2144,29 +2137,29 @@
       <c r="B18" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="39">
+      <c r="G18" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="31">
         <v>16.989999999999998</v>
       </c>
       <c r="I18" s="8">
         <v>2</v>
       </c>
       <c r="J18" s="11">
-        <f t="shared" ref="J18:J22" si="1">I18*H18</f>
+        <f t="shared" ref="J18:J22" si="2">I18*H18</f>
         <v>33.979999999999997</v>
       </c>
       <c r="K18" s="9"/>
@@ -2200,7 +2193,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.28</v>
       </c>
       <c r="K19" s="9"/>
@@ -2235,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4950000000000001</v>
       </c>
       <c r="K20" s="9"/>
@@ -2270,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.9950000000000001</v>
       </c>
       <c r="K21" s="9"/>
@@ -2291,20 +2284,20 @@
       <c r="E22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="37" t="s">
+      <c r="F22" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="H22" s="39">
+      <c r="H22" s="31">
         <v>2.5</v>
       </c>
       <c r="I22" s="8">
         <v>1</v>
       </c>
       <c r="J22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="K22" s="9" t="s">
@@ -2340,7 +2333,7 @@
       <c r="I23" s="8">
         <v>2</v>
       </c>
-      <c r="J23" s="48">
+      <c r="J23" s="40">
         <f>I23*H23</f>
         <v>7.333333333333333</v>
       </c>
@@ -2348,54 +2341,54 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>16</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="47">
+      <c r="H24" s="39">
         <v>1.2</v>
       </c>
-      <c r="I24" s="43">
+      <c r="I24" s="35">
         <v>4</v>
       </c>
-      <c r="J24" s="48">
+      <c r="J24" s="40">
         <f>I24*H24</f>
         <v>4.8</v>
       </c>
-      <c r="K24" s="45"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="24">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="23">
         <f xml:space="preserve"> SUM(J9:J24)</f>
         <v>492.65453333333335</v>
       </c>
@@ -2452,67 +2445,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="49">
         <v>43566</v>
       </c>
-      <c r="C3" s="29"/>
+      <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="29"/>
-    </row>
-    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="C4" s="49"/>
+    </row>
+    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="18"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -2651,7 +2644,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="11">
-        <f>I11*H11</f>
+        <f t="shared" ref="J11:J16" si="1">I11*H11</f>
         <v>3.7520000000000002</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -2688,7 +2681,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="11">
-        <f>I12*H12</f>
+        <f t="shared" si="1"/>
         <v>0.19519999999999998</v>
       </c>
       <c r="K12" s="9"/>
@@ -2722,7 +2715,7 @@
         <v>0.1</v>
       </c>
       <c r="J13" s="11">
-        <f>I13*H13</f>
+        <f t="shared" si="1"/>
         <v>1.3860000000000001</v>
       </c>
       <c r="K13" s="9"/>
@@ -2756,7 +2749,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="11">
-        <f>I14*H14</f>
+        <f t="shared" si="1"/>
         <v>25.94</v>
       </c>
       <c r="K14" s="9"/>
@@ -2791,10 +2784,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="11">
-        <f>I15*H15</f>
+        <f t="shared" si="1"/>
         <v>68.89</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="27" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2817,7 +2810,7 @@
       <c r="F16" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="34" t="s">
         <v>86</v>
       </c>
       <c r="H16" s="10">
@@ -2827,10 +2820,10 @@
         <v>0.1</v>
       </c>
       <c r="J16" s="11">
-        <f>I16*H16</f>
+        <f t="shared" si="1"/>
         <v>1.468</v>
       </c>
-      <c r="K16" s="28"/>
+      <c r="K16" s="27"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -2839,29 +2832,29 @@
       <c r="B17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="39">
+      <c r="G17" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="31">
         <v>16.989999999999998</v>
       </c>
       <c r="I17" s="8">
         <v>2</v>
       </c>
       <c r="J17" s="11">
-        <f t="shared" ref="J17:J21" si="1">I17*H17</f>
+        <f t="shared" ref="J17:J21" si="2">I17*H17</f>
         <v>33.979999999999997</v>
       </c>
       <c r="K17" s="9"/>
@@ -2895,7 +2888,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.28</v>
       </c>
       <c r="K18" s="9"/>
@@ -2930,7 +2923,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4950000000000001</v>
       </c>
       <c r="K19" s="9"/>
@@ -2965,7 +2958,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.9950000000000001</v>
       </c>
       <c r="K20" s="9"/>
@@ -2986,20 +2979,20 @@
       <c r="E21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="39">
+      <c r="H21" s="31">
         <v>2.5</v>
       </c>
       <c r="I21" s="8">
         <v>1</v>
       </c>
       <c r="J21" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="K21" s="9" t="s">
@@ -3035,7 +3028,7 @@
       <c r="I22" s="8">
         <v>2</v>
       </c>
-      <c r="J22" s="48">
+      <c r="J22" s="40">
         <f>I22*H22</f>
         <v>7.333333333333333</v>
       </c>
@@ -3072,7 +3065,7 @@
       <c r="I23" s="8">
         <v>0</v>
       </c>
-      <c r="J23" s="48">
+      <c r="J23" s="40">
         <f>I23*H23</f>
         <v>0</v>
       </c>
@@ -3080,54 +3073,54 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>17</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="47">
+      <c r="H24" s="39">
         <v>1.2</v>
       </c>
-      <c r="I24" s="43">
+      <c r="I24" s="35">
         <v>4</v>
       </c>
-      <c r="J24" s="48">
+      <c r="J24" s="40">
         <f>I24*H24</f>
         <v>4.8</v>
       </c>
-      <c r="K24" s="45"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="24">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="23">
         <f xml:space="preserve"> SUM(J9:J24)</f>
         <v>494.01453333333336</v>
       </c>
@@ -3165,8 +3158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3185,45 +3178,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="49">
         <v>43566</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="16"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="18"/>
+      <c r="C3" s="49"/>
+    </row>
+    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="15"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -3264,7 +3257,7 @@
       <c r="A7" s="8">
         <v>1</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>102</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -3282,14 +3275,14 @@
       <c r="G7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="31">
         <v>299</v>
       </c>
       <c r="I7" s="8">
         <v>1</v>
       </c>
       <c r="J7" s="11">
-        <f>I7*H7</f>
+        <f t="shared" ref="J7:J12" si="0">I7*H7</f>
         <v>299</v>
       </c>
       <c r="K7" s="9"/>
@@ -3298,7 +3291,7 @@
       <c r="A8" s="8">
         <v>2</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>107</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -3316,14 +3309,14 @@
       <c r="G8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="31">
         <v>55.58</v>
       </c>
       <c r="I8" s="8">
         <v>1</v>
       </c>
       <c r="J8" s="11">
-        <f>I8*H8</f>
+        <f t="shared" si="0"/>
         <v>55.58</v>
       </c>
       <c r="K8" s="9" t="s">
@@ -3334,7 +3327,7 @@
       <c r="A9" s="8">
         <v>3</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>108</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -3352,14 +3345,14 @@
       <c r="G9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="31">
         <v>64.430000000000007</v>
       </c>
       <c r="I9" s="8">
         <v>1</v>
       </c>
       <c r="J9" s="11">
-        <f>I9*H9</f>
+        <f t="shared" si="0"/>
         <v>64.430000000000007</v>
       </c>
       <c r="K9" s="9" t="s">
@@ -3370,7 +3363,7 @@
       <c r="A10" s="8">
         <v>4</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>106</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -3388,12 +3381,14 @@
       <c r="G10" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="31">
+        <v>0</v>
+      </c>
       <c r="I10" s="8">
         <v>0</v>
       </c>
       <c r="J10" s="11">
-        <f>I10*H10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10" s="9" t="s">
@@ -3404,7 +3399,7 @@
       <c r="A11" s="8">
         <v>5</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>109</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -3422,14 +3417,14 @@
       <c r="G11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="31">
         <v>77.73</v>
       </c>
       <c r="I11" s="8">
         <v>0</v>
       </c>
       <c r="J11" s="11">
-        <f>I11*H11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -3440,7 +3435,7 @@
       <c r="A12" s="8">
         <v>6</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>110</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -3458,14 +3453,14 @@
       <c r="G12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="31">
         <v>87.08</v>
       </c>
       <c r="I12" s="8">
         <v>0</v>
       </c>
       <c r="J12" s="11">
-        <f>I12*H12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12" s="9" t="s">
@@ -3473,31 +3468,31 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="51"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="43"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="24">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="23">
         <f>SUM(J7:J12)</f>
         <v>419.01</v>
       </c>

</xml_diff>